<commit_message>
Ajout du suivi de la comete C/2020 F3 (Neowise)
</commit_message>
<xml_diff>
--- a/Master_Telescope/Vitesse_Moteur.xlsx
+++ b/Master_Telescope/Vitesse_Moteur.xlsx
@@ -5,27 +5,27 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DIETRICHT_ELEC\Desktop\Diplome_Telescope_Dietrich_V33\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tanguy\Desktop\Astrophotography-Assistant-master\Master_Telescope\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="1185" windowWidth="25200" windowHeight="11880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="fCLK">Feuil1!$P$8</definedName>
-    <definedName name="modebit">Feuil1!$P$9</definedName>
-    <definedName name="modebitT0">Feuil1!$P$9</definedName>
-    <definedName name="ModeBitT4">Feuil1!$R$9</definedName>
-    <definedName name="Multiplicateur">Feuil1!$P$5</definedName>
-    <definedName name="Prediviseur">Feuil1!$P$7</definedName>
-    <definedName name="Prediviseur_T4">Feuil1!$R$7</definedName>
-    <definedName name="PrediviseurT0">Feuil1!$P$7</definedName>
-    <definedName name="Step_Angle">Feuil1!$P$3</definedName>
-    <definedName name="Step_Mode">Feuil1!$P$4</definedName>
-    <definedName name="tempo_T4">Feuil1!$R$10</definedName>
+    <definedName name="fCLK">Feuil1!$S$8</definedName>
+    <definedName name="modebit">Feuil1!$S$9</definedName>
+    <definedName name="modebitT0">Feuil1!$S$9</definedName>
+    <definedName name="ModeBitT4">Feuil1!$U$9</definedName>
+    <definedName name="Multiplicateur">Feuil1!$S$5</definedName>
+    <definedName name="Prediviseur">Feuil1!$S$7</definedName>
+    <definedName name="Prediviseur_T4">Feuil1!$U$7</definedName>
+    <definedName name="PrediviseurT0">Feuil1!$S$7</definedName>
+    <definedName name="Step_Angle">Feuil1!$S$3</definedName>
+    <definedName name="Step_Mode">Feuil1!$S$4</definedName>
+    <definedName name="tempo_T4">Feuil1!$U$10</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Temps de revolution</t>
   </si>
@@ -84,9 +84,6 @@
     <t>x16</t>
   </si>
   <si>
-    <t>x0,5</t>
-  </si>
-  <si>
     <t>x8</t>
   </si>
   <si>
@@ -139,6 +136,24 @@
   </si>
   <si>
     <t>x48</t>
+  </si>
+  <si>
+    <t>x0,4</t>
+  </si>
+  <si>
+    <t>xTest</t>
+  </si>
+  <si>
+    <t>C/2020 F3</t>
+  </si>
+  <si>
+    <t>Calcul comete</t>
+  </si>
+  <si>
+    <t>DeltaT</t>
+  </si>
+  <si>
+    <t>secondes</t>
   </si>
 </sst>
 </file>
@@ -174,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -188,6 +203,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,53 +518,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:R18"/>
+  <dimension ref="C3:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" customWidth="1"/>
+    <col min="7" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.875" customWidth="1"/>
-    <col min="16" max="16" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.375" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="14" max="14" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.875" customWidth="1"/>
+    <col min="19" max="19" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="O3" t="s">
+    <row r="3" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="1">
+      <c r="S3" s="1">
         <f>7.5</f>
         <v>7.5</v>
       </c>
     </row>
-    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="M4" t="s">
-        <v>32</v>
+    <row r="4" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f>86164-G6</f>
+        <v>3662</v>
       </c>
       <c r="O4" t="s">
+        <v>31</v>
+      </c>
+      <c r="R4" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>1</v>
@@ -565,26 +590,35 @@
       <c r="J5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="P5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" t="s">
         <v>10</v>
       </c>
-      <c r="P5">
+      <c r="S5">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -612,22 +646,34 @@
         <v>43082</v>
       </c>
       <c r="K6" s="2">
-        <f>F6/0.5</f>
-        <v>172328</v>
+        <f>F6/1.4</f>
+        <v>61545.71428571429</v>
       </c>
       <c r="L6" s="2">
+        <f>F6/0.6</f>
+        <v>143606.66666666669</v>
+      </c>
+      <c r="M6" s="2">
+        <f>F6/0.7</f>
+        <v>123091.42857142858</v>
+      </c>
+      <c r="N6" s="2">
         <f>F6/8</f>
         <v>10770.5</v>
       </c>
-      <c r="M6" s="2">
+      <c r="O6" s="2">
         <v>240</v>
       </c>
-      <c r="N6" s="2">
+      <c r="P6" s="2">
         <f>F6/48</f>
         <v>1795.0833333333333</v>
       </c>
-    </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="Q6" s="2">
+        <f>J25</f>
+        <v>85019</v>
+      </c>
+    </row>
+    <row r="7" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>5</v>
       </c>
@@ -652,7 +698,7 @@
         <v>4.1900904361185792E-3</v>
       </c>
       <c r="I7" s="5">
-        <f t="shared" ref="I7:M7" si="0">360/I6</f>
+        <f t="shared" ref="I7:O7" si="0">360/I6</f>
         <v>6.6849264193862862E-2</v>
       </c>
       <c r="J7" s="5">
@@ -660,35 +706,47 @@
         <v>8.3561580242328577E-3</v>
       </c>
       <c r="K7" s="5">
-        <f t="shared" si="0"/>
-        <v>2.0890395060582144E-3</v>
+        <f t="shared" ref="K7" si="1">360/K6</f>
+        <v>5.8493106169630006E-3</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="0"/>
+        <v>2.5068474072698571E-3</v>
+      </c>
+      <c r="M7" s="5">
+        <f t="shared" ref="M7" si="2">360/M6</f>
+        <v>2.9246553084815003E-3</v>
+      </c>
+      <c r="N7" s="5">
+        <f t="shared" si="0"/>
         <v>3.3424632096931431E-2</v>
       </c>
-      <c r="M7" s="5">
+      <c r="O7" s="5">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="N7" s="5">
-        <f t="shared" ref="N7" si="1">360/N6</f>
+      <c r="P7" s="5">
+        <f t="shared" ref="P7:Q7" si="3">360/P6</f>
         <v>0.20054779258158861</v>
       </c>
-      <c r="O7" t="s">
-        <v>17</v>
-      </c>
-      <c r="P7">
-        <v>48</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>19</v>
-      </c>
-      <c r="R7">
+      <c r="Q7" s="5">
+        <f t="shared" si="3"/>
+        <v>4.2343476164151544E-3</v>
+      </c>
+      <c r="R7" t="s">
+        <v>16</v>
+      </c>
+      <c r="S7">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T7" t="s">
+        <v>18</v>
+      </c>
+      <c r="U7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>4</v>
       </c>
@@ -705,45 +763,57 @@
         <v>15.041084443619145</v>
       </c>
       <c r="G8" s="5">
-        <f t="shared" ref="G8:H8" si="2">G7*3600</f>
+        <f t="shared" ref="G8:H8" si="4">G7*3600</f>
         <v>15.70871009187656</v>
       </c>
       <c r="H8" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>15.084325570026886</v>
       </c>
       <c r="I8" s="5">
-        <f t="shared" ref="I8" si="3">I7*3600</f>
+        <f t="shared" ref="I8" si="5">I7*3600</f>
         <v>240.65735109790631</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" ref="J8" si="4">J7*3600</f>
+        <f t="shared" ref="J8:K8" si="6">J7*3600</f>
         <v>30.082168887238289</v>
       </c>
       <c r="K8" s="5">
-        <f t="shared" ref="K8" si="5">K7*3600</f>
-        <v>7.5205422218095723</v>
+        <f t="shared" si="6"/>
+        <v>21.0575182210668</v>
       </c>
       <c r="L8" s="5">
-        <f t="shared" ref="L8" si="6">L7*3600</f>
+        <f t="shared" ref="L8:M8" si="7">L7*3600</f>
+        <v>9.0246506661714854</v>
+      </c>
+      <c r="M8" s="5">
+        <f t="shared" si="7"/>
+        <v>10.5287591105334</v>
+      </c>
+      <c r="N8" s="5">
+        <f t="shared" ref="N8" si="8">N7*3600</f>
         <v>120.32867554895316</v>
       </c>
-      <c r="M8" s="5">
-        <f t="shared" ref="M8:N8" si="7">M7*3600</f>
+      <c r="O8" s="5">
+        <f t="shared" ref="O8:P8" si="9">O7*3600</f>
         <v>5400</v>
       </c>
-      <c r="N8" s="5">
-        <f t="shared" si="7"/>
+      <c r="P8" s="5">
+        <f t="shared" si="9"/>
         <v>721.972053293719</v>
       </c>
-      <c r="O8" t="s">
+      <c r="Q8" s="5">
+        <f t="shared" ref="Q8" si="10">Q7*3600</f>
+        <v>15.243651419094556</v>
+      </c>
+      <c r="R8" t="s">
         <v>11</v>
       </c>
-      <c r="P8">
+      <c r="S8">
         <v>48000000</v>
       </c>
     </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>3</v>
       </c>
@@ -760,53 +830,65 @@
         <v>0.60164337774476573</v>
       </c>
       <c r="G9" s="5">
-        <f t="shared" ref="G9:H9" si="8">G7*144</f>
+        <f t="shared" ref="G9:H9" si="11">G7*144</f>
         <v>0.62834840367506239</v>
       </c>
       <c r="H9" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.60337302280107541</v>
       </c>
       <c r="I9" s="5">
-        <f t="shared" ref="I9:M9" si="9">I7*144</f>
+        <f t="shared" ref="I9:O9" si="12">I7*144</f>
         <v>9.6262940439162517</v>
       </c>
       <c r="J9" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>1.2032867554895315</v>
       </c>
       <c r="K9" s="5">
-        <f t="shared" si="9"/>
-        <v>0.30082168887238286</v>
+        <f t="shared" ref="K9" si="13">K7*144</f>
+        <v>0.84230072884267204</v>
       </c>
       <c r="L9" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
+        <v>0.36098602664685941</v>
+      </c>
+      <c r="M9" s="5">
+        <f t="shared" ref="M9" si="14">M7*144</f>
+        <v>0.42115036442133602</v>
+      </c>
+      <c r="N9" s="5">
+        <f t="shared" si="12"/>
         <v>4.8131470219581258</v>
       </c>
-      <c r="M9" s="5">
-        <f t="shared" si="9"/>
+      <c r="O9" s="5">
+        <f t="shared" si="12"/>
         <v>216</v>
       </c>
-      <c r="N9" s="5">
-        <f t="shared" ref="N9" si="10">N7*144</f>
+      <c r="P9" s="5">
+        <f t="shared" ref="P9:Q9" si="15">P7*144</f>
         <v>28.87888213174876</v>
       </c>
-      <c r="O9" t="s">
-        <v>18</v>
-      </c>
-      <c r="P9">
+      <c r="Q9" s="5">
+        <f t="shared" si="15"/>
+        <v>0.60974605676378224</v>
+      </c>
+      <c r="R9" t="s">
+        <v>17</v>
+      </c>
+      <c r="S9">
         <v>16</v>
       </c>
-      <c r="Q9" t="s">
-        <v>20</v>
-      </c>
-      <c r="R9">
+      <c r="T9" t="s">
+        <v>19</v>
+      </c>
+      <c r="U9">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="5">
         <f>D9/360</f>
@@ -821,47 +903,59 @@
         <v>1.6712316048465715E-3</v>
       </c>
       <c r="G10" s="5">
-        <f t="shared" ref="G10:M10" si="11">G9/360</f>
+        <f t="shared" ref="G10:O10" si="16">G9/360</f>
         <v>1.745412232430729E-3</v>
       </c>
       <c r="H10" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.6760361744474316E-3</v>
       </c>
       <c r="I10" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>2.6739705677545144E-2</v>
       </c>
       <c r="J10" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>3.342463209693143E-3</v>
       </c>
       <c r="K10" s="5">
-        <f t="shared" si="11"/>
-        <v>8.3561580242328575E-4</v>
+        <f t="shared" ref="K10" si="17">K9/360</f>
+        <v>2.3397242467852E-3</v>
       </c>
       <c r="L10" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
+        <v>1.0027389629079428E-3</v>
+      </c>
+      <c r="M10" s="5">
+        <f t="shared" ref="M10" si="18">M9/360</f>
+        <v>1.1698621233926E-3</v>
+      </c>
+      <c r="N10" s="5">
+        <f t="shared" si="16"/>
         <v>1.3369852838772572E-2</v>
       </c>
-      <c r="M10" s="5">
-        <f t="shared" si="11"/>
+      <c r="O10" s="5">
+        <f t="shared" si="16"/>
         <v>0.6</v>
       </c>
-      <c r="N10" s="5">
-        <f t="shared" ref="N10" si="12">N9/360</f>
+      <c r="P10" s="5">
+        <f t="shared" ref="P10:Q10" si="19">P9/360</f>
         <v>8.0219117032635442E-2</v>
       </c>
-      <c r="Q10" t="s">
-        <v>25</v>
-      </c>
-      <c r="R10" s="4">
+      <c r="Q10" s="5">
+        <f t="shared" si="19"/>
+        <v>1.6937390465660619E-3</v>
+      </c>
+      <c r="T10" t="s">
+        <v>24</v>
+      </c>
+      <c r="U10" s="4">
         <v>5.4100000000000003E-4</v>
       </c>
     </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="5">
         <f>D10*60</f>
@@ -876,90 +970,114 @@
         <v>0.10027389629079429</v>
       </c>
       <c r="G11" s="5">
-        <f t="shared" ref="G11:M11" si="13">G10*60</f>
+        <f t="shared" ref="G11:O11" si="20">G10*60</f>
         <v>0.10472473394584374</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>0.1005621704668459</v>
       </c>
       <c r="I11" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>1.6043823406527087</v>
       </c>
       <c r="J11" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>0.20054779258158859</v>
       </c>
       <c r="K11" s="5">
-        <f t="shared" si="13"/>
-        <v>5.0136948145397146E-2</v>
+        <f t="shared" ref="K11" si="21">K10*60</f>
+        <v>0.14038345480711201</v>
       </c>
       <c r="L11" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
+        <v>6.0164337774476571E-2</v>
+      </c>
+      <c r="M11" s="5">
+        <f t="shared" ref="M11" si="22">M10*60</f>
+        <v>7.0191727403556003E-2</v>
+      </c>
+      <c r="N11" s="5">
+        <f t="shared" si="20"/>
         <v>0.80219117032635434</v>
       </c>
-      <c r="M11" s="5">
-        <f t="shared" si="13"/>
+      <c r="O11" s="5">
+        <f t="shared" si="20"/>
         <v>36</v>
       </c>
-      <c r="N11" s="5">
-        <f t="shared" ref="N11" si="14">N10*60</f>
+      <c r="P11" s="5">
+        <f t="shared" ref="P11:Q11" si="23">P10*60</f>
         <v>4.8131470219581267</v>
       </c>
-    </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="Q11" s="5">
+        <f t="shared" si="23"/>
+        <v>0.10162434279396371</v>
+      </c>
+    </row>
+    <row r="12" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="3">
         <f>(D17*360*Step_Mode)/(60*Step_Angle)</f>
-        <v>19.259919750334376</v>
+        <v>77.039679001337504</v>
       </c>
       <c r="E12" s="3">
         <f>(E17*360*Step_Mode)/(60*Step_Angle)</f>
-        <v>19.25562736795186</v>
+        <v>77.022509471807439</v>
       </c>
       <c r="F12" s="3">
         <f>(F17*360*Step_Mode)/(60*Step_Angle)</f>
-        <v>19.252588087832503</v>
+        <v>77.010352351330013</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" ref="G12:N12" si="15">(G17*360*Step_Mode)/(60*Step_Angle)</f>
-        <v>20.107148917601997</v>
+        <f t="shared" ref="G12:P12" si="24">(G17*360*Step_Mode)/(60*Step_Angle)</f>
+        <v>80.428595670407987</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" si="15"/>
-        <v>19.307936729634413</v>
+        <f t="shared" si="24"/>
+        <v>77.231746918537652</v>
       </c>
       <c r="I12" s="3">
-        <f t="shared" si="15"/>
-        <v>308.04140940532005</v>
+        <f t="shared" si="24"/>
+        <v>1232.1656376212802</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" si="15"/>
-        <v>38.505176175665007</v>
+        <f t="shared" si="24"/>
+        <v>154.02070470266003</v>
       </c>
       <c r="K12" s="3">
-        <f t="shared" si="15"/>
-        <v>9.6262940439162517</v>
+        <f t="shared" ref="K12" si="25">(K17*360*Step_Mode)/(60*Step_Angle)</f>
+        <v>107.81449329186204</v>
       </c>
       <c r="L12" s="3">
-        <f t="shared" si="15"/>
-        <v>154.02070470266003</v>
+        <f t="shared" si="24"/>
+        <v>46.206211410798005</v>
       </c>
       <c r="M12" s="3">
-        <f t="shared" si="15"/>
-        <v>6912</v>
+        <f t="shared" ref="M12" si="26">(M17*360*Step_Mode)/(60*Step_Angle)</f>
+        <v>53.907246645931018</v>
       </c>
       <c r="N12" s="3">
-        <f t="shared" si="15"/>
-        <v>924.12422821596033</v>
-      </c>
-    </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="24"/>
+        <v>616.08281881064011</v>
+      </c>
+      <c r="O12" s="3">
+        <f t="shared" si="24"/>
+        <v>27648</v>
+      </c>
+      <c r="P12" s="3">
+        <f t="shared" si="24"/>
+        <v>3696.4969128638413</v>
+      </c>
+      <c r="Q12" s="3">
+        <f t="shared" ref="Q12" si="27">(Q17*360*Step_Mode)/(60*Step_Angle)</f>
+        <v>78.047495265764141</v>
+      </c>
+    </row>
+    <row r="13" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="3">
         <f>POWER(2,modebit)-(((1/D12)/2)/(Prediviseur/fCLK))</f>
@@ -974,188 +1092,236 @@
         <v>39565.465663580238</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" ref="G13:N13" si="16">POWER(2,modebit)-(((1/G12)/2)/(Prediviseur/fCLK))</f>
+        <f t="shared" ref="G13:P13" si="28">POWER(2,modebit)-(((1/G12)/2)/(Prediviseur/fCLK))</f>
         <v>40669.222415123455</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="28"/>
         <v>39639.913483796292</v>
       </c>
       <c r="I13" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="28"/>
         <v>63912.841603973764</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="28"/>
         <v>52550.732831790119</v>
       </c>
       <c r="K13" s="3">
-        <f t="shared" si="16"/>
-        <v>13594.931327160484</v>
+        <f t="shared" ref="K13" si="29">POWER(2,modebit)-(((1/K12)/2)/(Prediviseur/fCLK))</f>
+        <v>46985.618331128746</v>
       </c>
       <c r="L13" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="28"/>
+        <v>22251.776105967074</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" ref="M13" si="30">POWER(2,modebit)-(((1/M12)/2)/(Prediviseur/fCLK))</f>
+        <v>28435.236662257499</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="28"/>
         <v>62289.683207947528</v>
       </c>
-      <c r="M13" s="3">
-        <f t="shared" si="16"/>
+      <c r="O13" s="3">
+        <f t="shared" si="28"/>
         <v>65463.662037037036</v>
       </c>
-      <c r="N13" s="3">
-        <f t="shared" si="16"/>
+      <c r="P13" s="3">
+        <f t="shared" si="28"/>
         <v>64994.94720132459</v>
       </c>
-    </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="Q13" s="3">
+        <f t="shared" ref="Q13" si="31">POWER(2,modebit)-(((1/Q12)/2)/(Prediviseur/fCLK))</f>
+        <v>39910.578028549389</v>
+      </c>
+    </row>
+    <row r="14" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="3">
         <f>POWER(2,ModeBitT4)-(((1/D12)/2)/(Prediviseur_T4/fCLK))</f>
-        <v>-38306.592592592584</v>
+        <v>39575.351851851854</v>
       </c>
       <c r="E14" s="3">
         <f>POWER(2,ModeBitT4)-(((1/E12)/2)/(Prediviseur_T4/fCLK))</f>
-        <v>-38329.740740740745</v>
+        <v>39569.564814814818</v>
       </c>
       <c r="F14" s="3">
         <f>POWER(2,ModeBitT4)-(((1/F12)/2)/(Prediviseur_T4/fCLK))</f>
-        <v>-38346.137345679032</v>
+        <v>39565.465663580238</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" ref="G14:N14" si="17">POWER(2,ModeBitT4)-(((1/G12)/2)/(Prediviseur_T4/fCLK))</f>
-        <v>-33931.11033950618</v>
+        <f t="shared" ref="G14:P14" si="32">POWER(2,ModeBitT4)-(((1/G12)/2)/(Prediviseur_T4/fCLK))</f>
+        <v>40669.222415123455</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="17"/>
-        <v>-38048.346064814832</v>
+        <f t="shared" si="32"/>
+        <v>39639.913483796292</v>
       </c>
       <c r="I14" s="3">
-        <f t="shared" si="17"/>
-        <v>59043.366415895063</v>
+        <f t="shared" si="32"/>
+        <v>63912.841603973764</v>
       </c>
       <c r="J14" s="3">
-        <f t="shared" si="17"/>
-        <v>13594.931327160484</v>
+        <f t="shared" si="32"/>
+        <v>52550.732831790119</v>
       </c>
       <c r="K14" s="3">
-        <f t="shared" si="17"/>
-        <v>-142228.27469135806</v>
+        <f t="shared" ref="K14" si="33">POWER(2,ModeBitT4)-(((1/K12)/2)/(Prediviseur_T4/fCLK))</f>
+        <v>46985.618331128746</v>
       </c>
       <c r="L14" s="3">
-        <f t="shared" si="17"/>
-        <v>52550.732831790119</v>
+        <f t="shared" si="32"/>
+        <v>22251.776105967074</v>
       </c>
       <c r="M14" s="3">
-        <f t="shared" si="17"/>
-        <v>65246.648148148146</v>
+        <f t="shared" ref="M14" si="34">POWER(2,ModeBitT4)-(((1/M12)/2)/(Prediviseur_T4/fCLK))</f>
+        <v>28435.236662257499</v>
       </c>
       <c r="N14" s="3">
-        <f t="shared" si="17"/>
-        <v>63371.788805298354</v>
-      </c>
-    </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="32"/>
+        <v>62289.683207947528</v>
+      </c>
+      <c r="O14" s="3">
+        <f t="shared" si="32"/>
+        <v>65463.662037037036</v>
+      </c>
+      <c r="P14" s="3">
+        <f t="shared" si="32"/>
+        <v>64994.94720132459</v>
+      </c>
+      <c r="Q14" s="3">
+        <f t="shared" ref="Q14" si="35">POWER(2,ModeBitT4)-(((1/Q12)/2)/(Prediviseur_T4/fCLK))</f>
+        <v>39910.578028549389</v>
+      </c>
+    </row>
+    <row r="15" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="5">
         <f>(1/D12)/2</f>
-        <v>2.5960648148148146E-2</v>
+        <v>6.4901620370370365E-3</v>
       </c>
       <c r="E15" s="5">
         <f>(1/E12)/2</f>
-        <v>2.5966435185185186E-2</v>
+        <v>6.4916087962962965E-3</v>
       </c>
       <c r="F15" s="6">
         <f>(1/F12)/2</f>
-        <v>2.5970534336419757E-2</v>
+        <v>6.4926335841049392E-3</v>
       </c>
       <c r="G15" s="6">
-        <f t="shared" ref="G15:J15" si="18">(1/G12)/2</f>
-        <v>2.4866777584876543E-2</v>
+        <f t="shared" ref="G15:J15" si="36">(1/G12)/2</f>
+        <v>6.2166943962191357E-3</v>
       </c>
       <c r="H15" s="6">
-        <f t="shared" si="18"/>
-        <v>2.5896086516203707E-2</v>
+        <f t="shared" si="36"/>
+        <v>6.4740216290509267E-3</v>
       </c>
       <c r="I15" s="6">
-        <f t="shared" si="18"/>
-        <v>1.6231583960262348E-3</v>
+        <f t="shared" si="36"/>
+        <v>4.057895990065587E-4</v>
       </c>
       <c r="J15" s="6">
-        <f t="shared" si="18"/>
-        <v>1.2985267168209878E-2</v>
+        <f t="shared" si="36"/>
+        <v>3.2463167920524696E-3</v>
       </c>
       <c r="K15" s="6">
-        <f>(1/K12)/2</f>
-        <v>5.1941068672839513E-2</v>
+        <f t="shared" ref="K15" si="37">(1/K12)/2</f>
+        <v>4.6375954172178128E-3</v>
       </c>
       <c r="L15" s="6">
-        <f t="shared" ref="L15:N15" si="19">(1/L12)/2</f>
-        <v>3.2463167920524696E-3</v>
+        <f>(1/L12)/2</f>
+        <v>1.0821055973508232E-2</v>
       </c>
       <c r="M15" s="6">
-        <f t="shared" si="19"/>
-        <v>7.2337962962962959E-5</v>
+        <f>(1/M12)/2</f>
+        <v>9.2751908344356256E-3</v>
       </c>
       <c r="N15" s="6">
-        <f t="shared" si="19"/>
-        <v>5.4105279867541149E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" ref="N15:P15" si="38">(1/N12)/2</f>
+        <v>8.1157919801311739E-4</v>
+      </c>
+      <c r="O15" s="6">
+        <f t="shared" si="38"/>
+        <v>1.808449074074074E-5</v>
+      </c>
+      <c r="P15" s="6">
+        <f t="shared" si="38"/>
+        <v>1.3526319966885287E-4</v>
+      </c>
+      <c r="Q15" s="6">
+        <f t="shared" ref="Q15" si="39">(1/Q12)/2</f>
+        <v>6.4063554928626525E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="5">
         <f>D15/tempo_T4</f>
-        <v>47.98641062504278</v>
+        <v>11.996602656260695</v>
       </c>
       <c r="E16" s="5">
         <f>E15/tempo_T4</f>
-        <v>47.997107551174096</v>
+        <v>11.999276887793524</v>
       </c>
       <c r="F16" s="6">
         <f>F15/tempo_T4</f>
-        <v>48.004684540517104</v>
+        <v>12.001171135129276</v>
       </c>
       <c r="G16" s="6">
-        <f t="shared" ref="G16:N16" si="20">G15/tempo_T4</f>
-        <v>45.964468733598046</v>
+        <f t="shared" ref="G16:P16" si="40">G15/tempo_T4</f>
+        <v>11.491117183399512</v>
       </c>
       <c r="H16" s="6">
-        <f t="shared" si="20"/>
-        <v>47.867073042890397</v>
+        <f t="shared" si="40"/>
+        <v>11.966768260722599</v>
       </c>
       <c r="I16" s="6">
-        <f t="shared" si="20"/>
-        <v>3.000292783782319</v>
+        <f t="shared" si="40"/>
+        <v>0.75007319594557975</v>
       </c>
       <c r="J16" s="6">
-        <f t="shared" si="20"/>
-        <v>24.002342270258552</v>
+        <f t="shared" si="40"/>
+        <v>6.000585567564638</v>
       </c>
       <c r="K16" s="6">
-        <f t="shared" si="20"/>
-        <v>96.009369081034208</v>
+        <f t="shared" ref="K16" si="41">K15/tempo_T4</f>
+        <v>8.5722650965209102</v>
       </c>
       <c r="L16" s="6">
-        <f t="shared" si="20"/>
-        <v>6.000585567564638</v>
+        <f t="shared" si="40"/>
+        <v>20.001951891882129</v>
       </c>
       <c r="M16" s="6">
-        <f t="shared" si="20"/>
-        <v>0.13371157664133634</v>
+        <f t="shared" ref="M16" si="42">M15/tempo_T4</f>
+        <v>17.14453019304182</v>
       </c>
       <c r="N16" s="6">
-        <f t="shared" si="20"/>
-        <v>1.0000975945941062</v>
-      </c>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="40"/>
+        <v>1.5001463918911595</v>
+      </c>
+      <c r="O16" s="6">
+        <f t="shared" si="40"/>
+        <v>3.3427894160334086E-2</v>
+      </c>
+      <c r="P16" s="6">
+        <f t="shared" si="40"/>
+        <v>0.25002439864852655</v>
+      </c>
+      <c r="Q16" s="6">
+        <f t="shared" ref="Q16" si="43">Q15/tempo_T4</f>
+        <v>11.841692223406012</v>
+      </c>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="5">
         <f>D11*Multiplicateur</f>
@@ -1170,41 +1336,53 @@
         <v>12.032867554895315</v>
       </c>
       <c r="G17" s="6">
-        <f t="shared" ref="G17:N17" si="21">G11*Multiplicateur</f>
+        <f t="shared" ref="G17:P17" si="44">G11*Multiplicateur</f>
         <v>12.566968073501249</v>
       </c>
       <c r="H17" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="44"/>
         <v>12.067460456021507</v>
       </c>
       <c r="I17" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="44"/>
         <v>192.52588087832504</v>
       </c>
       <c r="J17" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="44"/>
         <v>24.06573510979063</v>
       </c>
       <c r="K17" s="6">
-        <f t="shared" si="21"/>
-        <v>6.0164337774476575</v>
+        <f t="shared" ref="K17" si="45">K11*Multiplicateur</f>
+        <v>16.846014576853442</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="44"/>
+        <v>7.2197205329371883</v>
+      </c>
+      <c r="M17" s="6">
+        <f t="shared" ref="M17" si="46">M11*Multiplicateur</f>
+        <v>8.4230072884267209</v>
+      </c>
+      <c r="N17" s="6">
+        <f t="shared" si="44"/>
         <v>96.26294043916252</v>
       </c>
-      <c r="M17" s="6">
-        <f t="shared" si="21"/>
+      <c r="O17" s="6">
+        <f t="shared" si="44"/>
         <v>4320</v>
       </c>
-      <c r="N17" s="6">
-        <f t="shared" si="21"/>
+      <c r="P17" s="6">
+        <f t="shared" si="44"/>
         <v>577.57764263497518</v>
       </c>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="Q17" s="6">
+        <f t="shared" ref="Q17" si="47">Q11*Multiplicateur</f>
+        <v>12.194921135275646</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="5">
         <f>D10*Multiplicateur</f>
@@ -1219,36 +1397,87 @@
         <v>0.20054779258158859</v>
       </c>
       <c r="G18" s="6">
-        <f t="shared" ref="G18:N18" si="22">G10*Multiplicateur</f>
+        <f t="shared" ref="G18:P18" si="48">G10*Multiplicateur</f>
         <v>0.20944946789168747</v>
       </c>
       <c r="H18" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="48"/>
         <v>0.2011243409336918</v>
       </c>
       <c r="I18" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="48"/>
         <v>3.2087646813054174</v>
       </c>
       <c r="J18" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="48"/>
         <v>0.40109558516317717</v>
       </c>
       <c r="K18" s="6">
-        <f t="shared" si="22"/>
-        <v>0.10027389629079429</v>
+        <f t="shared" ref="K18" si="49">K10*Multiplicateur</f>
+        <v>0.28076690961422401</v>
       </c>
       <c r="L18" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="48"/>
+        <v>0.12032867554895314</v>
+      </c>
+      <c r="M18" s="6">
+        <f t="shared" ref="M18" si="50">M10*Multiplicateur</f>
+        <v>0.14038345480711201</v>
+      </c>
+      <c r="N18" s="6">
+        <f t="shared" si="48"/>
         <v>1.6043823406527087</v>
       </c>
-      <c r="M18" s="6">
-        <f t="shared" si="22"/>
+      <c r="O18" s="6">
+        <f t="shared" si="48"/>
         <v>72</v>
       </c>
-      <c r="N18" s="6">
-        <f t="shared" si="22"/>
+      <c r="P18" s="6">
+        <f t="shared" si="48"/>
         <v>9.6262940439162534</v>
+      </c>
+      <c r="Q18" s="6">
+        <f t="shared" ref="Q18" si="51">Q10*Multiplicateur</f>
+        <v>0.20324868558792741</v>
+      </c>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="I23" s="7">
+        <v>44023</v>
+      </c>
+      <c r="J23">
+        <v>121846</v>
+      </c>
+      <c r="K23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="I24" s="7">
+        <v>44022</v>
+      </c>
+      <c r="J24">
+        <v>36827</v>
+      </c>
+      <c r="K24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J25">
+        <f>J23-J24</f>
+        <v>85019</v>
+      </c>
+      <c r="K25" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>